<commit_message>
blogs are finally done
</commit_message>
<xml_diff>
--- a/blog/blog_list.xlsx
+++ b/blog/blog_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clients\Myriad Communications\website 2018\txt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\mediamavenscg\PROJECTS\mattglowacki_2018-02\blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FBF2CE-BCE8-4A26-A2F1-EFE5E57BAC54}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="8415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>filename</t>
   </si>
@@ -59,12 +60,6 @@
     <t>2017_12_17.blog</t>
   </si>
   <si>
-    <t>Should I Say “Walk”?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You won’t offend me by saying “walk.” </t>
-  </si>
-  <si>
     <t>Your Name Can Be a Disability</t>
   </si>
   <si>
@@ -81,12 +76,24 @@
   </si>
   <si>
     <t>Some people just have a lack of self-awareness, not malicousness.</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Should I Say 'Walk?'</t>
+  </si>
+  <si>
+    <t>You won't offend me by saying 'Walk.'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,9 +129,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,106 +457,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.46484375" customWidth="1"/>
-    <col min="2" max="2" width="29.59765625" customWidth="1"/>
-    <col min="3" max="3" width="85.19921875" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="85.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2">
+        <v>43135</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2">
+        <v>43106</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2">
+        <v>43086</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43075</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.6">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43053</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.6">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>